<commit_message>
fix: fixed refresh document for xlsx
</commit_message>
<xml_diff>
--- a/upload-test-data/test.xlsx
+++ b/upload-test-data/test.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\matthias\Development\learning\alfresco\upload-test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0E2898-DD0F-4A80-8D5C-2779E5D1D90B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA7FE138-5BDF-4ABE-96CD-94E6B6C662A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{C3C00633-610E-4731-8FF9-C452F6E2DDCF}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="27240" windowHeight="15225" xr2:uid="{C3C00633-610E-4731-8FF9-C452F6E2DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>asdfasdfasdf</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>yxcv</t>
+  </si>
+  <si>
+    <t>NEW CHANGE</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A6:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +449,11 @@
         <v>1</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
chore: update testdata, vscode task fixes
</commit_message>
<xml_diff>
--- a/upload-test-data/test.xlsx
+++ b/upload-test-data/test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\matthias\Development\learning\alfresco\upload-test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6309CD38-4C03-44F5-B13A-76311871C870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9371E0-14A6-40A1-9D6D-16F86940EEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39880" yWindow="1620" windowWidth="28800" windowHeight="15450" xr2:uid="{C3C00633-610E-4731-8FF9-C452F6E2DDCF}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="28800" windowHeight="15345" xr2:uid="{C3C00633-610E-4731-8FF9-C452F6E2DDCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,27 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>asdfasdfasdf</t>
-  </si>
-  <si>
-    <t>yxcvyxcv</t>
-  </si>
-  <si>
-    <t>yxcv</t>
-  </si>
-  <si>
-    <t>NEW CHANGE</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>asdfasdf</t>
-  </si>
-  <si>
-    <t>asdsf</t>
   </si>
 </sst>
 </file>
@@ -428,15 +410,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B9FA6B-3F15-4BA1-B89B-4E4DCC2B6936}">
-  <dimension ref="A6:G24"/>
+  <dimension ref="A6:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>123123</v>
       </c>
@@ -453,39 +435,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="F7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C14" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="G18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="E24" t="s">
-        <v>5</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>851</v>
       </c>
     </row>
   </sheetData>

</xml_diff>